<commit_message>
optimize the test process
</commit_message>
<xml_diff>
--- a/hdmi_hdbt_test_suite/ConfigResolutionData.xlsx
+++ b/hdmi_hdbt_test_suite/ConfigResolutionData.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ResolutionData" sheetId="1" r:id="rId1"/>
     <sheet name="DUTConfig" sheetId="2" r:id="rId2"/>
+    <sheet name="ColorSpace" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" refMode="R1C1"/>
 </workbook>
@@ -33,6 +34,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Default:HDMI1
@@ -48,6 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="宋体"/>
+            <family val="3"/>
             <charset val="134"/>
           </rPr>
           <t>Default:HDMI1
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10090" uniqueCount="1459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10273" uniqueCount="1499">
   <si>
     <t>CODE</t>
   </si>
@@ -4535,10 +4538,6 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>HDMI1:1,HDMI2:2,HDMI3:3,HDMI4:4,HDBT1:3</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <t>CVT1960D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4553,6 +4552,321 @@
   <si>
     <t>2160p50w</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GB</t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lack</t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>White</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGB</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr444</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr422</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colorimetry</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uto</t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr420</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x10', '0x10', '0x10']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x10', '0x80', '0x10']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr422</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGB</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>4K</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>HDMI1:8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,HDMI2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,HDMI3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,HDMI4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,HDBT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x15', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x1C', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x15', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0x16']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0xFF']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xFF', '0xFF', '0xFF']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x13', '0x13', '0x13']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x07', '0x07', '0x07']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>InColorSpace</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutColorSpace</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGB</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr444</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr444</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGB</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x0A', '0x0A', '0x0A']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFE', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0xF7']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xF7', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFE', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFE', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFE', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0xFF']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4570,12 +4884,14 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4583,6 +4899,7 @@
       <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="major"/>
     </font>
@@ -4591,6 +4908,7 @@
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4599,6 +4917,7 @@
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4607,6 +4926,7 @@
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4614,6 +4934,7 @@
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4621,6 +4942,7 @@
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4628,6 +4950,7 @@
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4635,6 +4958,7 @@
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4643,6 +4967,7 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4651,6 +4976,7 @@
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4658,6 +4984,7 @@
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4666,6 +4993,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4673,6 +5001,7 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4681,6 +5010,7 @@
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4689,6 +5019,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4696,6 +5027,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4710,6 +5042,7 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4718,6 +5051,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -4914,7 +5248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -5026,6 +5360,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5158,7 +5507,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5190,6 +5539,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5521,11 +5879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO480"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="15" topLeftCell="K460" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="N471" sqref="N471"/>
+    <sheetView topLeftCell="A442" workbookViewId="0">
+      <selection activeCell="AL82" sqref="AL82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -5540,61 +5895,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>1404</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
       <c r="AB1" t="s">
         <v>1405</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="14" t="s">
         <v>1406</v>
       </c>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
       <c r="AJ1" t="s">
         <v>1405</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AK1" s="14" t="s">
         <v>1407</v>
       </c>
-      <c r="AL1" s="11"/>
+      <c r="AL1" s="14"/>
       <c r="AM1" t="s">
         <v>1405</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AN1" s="15" t="s">
         <v>1434</v>
       </c>
-      <c r="AO1" s="11"/>
+      <c r="AO1" s="14"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -14311,7 +14666,7 @@
         <v>30</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="D82" t="s">
         <v>268</v>
@@ -45828,7 +46183,7 @@
         <v>30</v>
       </c>
       <c r="C371" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="D371" t="s">
         <v>1100</v>
@@ -56289,7 +56644,7 @@
         <v>30</v>
       </c>
       <c r="C470" s="5" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="D470" t="s">
         <v>1390</v>
@@ -56500,7 +56855,7 @@
         <v>30</v>
       </c>
       <c r="C472" s="5" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="D472" t="s">
         <v>1394</v>
@@ -56628,7 +56983,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -56729,8 +57084,8 @@
       <c r="A12" s="5" t="s">
         <v>1418</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>1454</v>
+      <c r="B12" s="11" t="s">
+        <v>1473</v>
       </c>
     </row>
   </sheetData>
@@ -56739,4 +57094,692 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="27.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>1471</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1483</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>1464</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>1459</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>1470</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>1467</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>1470</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>1467</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>1480</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>1458</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>1476</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>1474</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>1481</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>1488</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>1474</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>1489</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>1487</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>1481</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13" t="s">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>1468</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>1490</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13" t="s">
+        <v>1462</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13" t="s">
+        <v>1497</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>1468</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>1466</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix some bug about VideoTestSuite
</commit_message>
<xml_diff>
--- a/hdmi_hdbt_test_suite/ConfigResolutionData.xlsx
+++ b/hdmi_hdbt_test_suite/ConfigResolutionData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ResolutionData" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10281" uniqueCount="1507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10380" uniqueCount="1561">
   <si>
     <t>CODE</t>
   </si>
@@ -4369,10 +4369,6 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>192.168.2.121</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <t>test1</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
@@ -4526,10 +4522,6 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>192.168.2.101</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <t>CVT1960D</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4580,10 +4572,6 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>White</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <t>RGB</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
@@ -4645,8 +4633,136 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
+    <t>['0x80', '0x15', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x1C', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x15', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0x16']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0xFF']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xFF', '0xFF', '0xFF']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x13', '0x13', '0x13']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x07', '0x07', '0x07']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>InColorSpace</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>OutColorSpace</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGB</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr444</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr444</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGB</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x0A', '0x0A', '0x0A']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFE', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0xF7']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xF7', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFE', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFE', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFE', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0xFF']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>ConfigResolutionData.xlsx</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x10', '0x10', '0x11']</t>
+  </si>
+  <si>
+    <t>['0x0A', '0x0A', '0x1A']</t>
+  </si>
+  <si>
+    <t>['0x13', '0x13', '0x14']</t>
+  </si>
+  <si>
+    <t>['0x80', '0x15', '0x81']</t>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0x17']</t>
+  </si>
+  <si>
+    <t>['0x07', '0x07', '0x08']</t>
+  </si>
+  <si>
+    <t>['0x80', '0x1C', '0x81']</t>
+  </si>
+  <si>
+    <t>['0x10', '0x80', '0x11']</t>
+  </si>
+  <si>
     <r>
-      <t>HDMI1:8</t>
+      <t>192.168.</t>
     </r>
     <r>
       <rPr>
@@ -4657,7 +4773,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,HDMI2:</t>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -4668,7 +4784,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>9</t>
+      <t>.</t>
     </r>
     <r>
       <rPr>
@@ -4679,7 +4795,13 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,HDMI3:</t>
+      <t>240</t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>192.168.</t>
     </r>
     <r>
       <rPr>
@@ -4690,207 +4812,237 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,HDMI4:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,HDBT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10</t>
+      <t>1.241</t>
     </r>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
+    <t>32002:1:1</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>HDMI1:1,HDMI2:2,HDMI3:3,HDMI4:4,HDBT3:3</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
     <t>['0x80', '0x15', '0x80']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0x1C', '0x80']</t>
+    <t>White</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0x15', '0x80']</t>
+    <t>Red</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0x80', '0x16']</t>
+    <t>['0xFF', '0x00', '0x0F']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0x80', '0xFF']</t>
+    <t>['0xFF', '0x00', '0x0F']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0xFF', '0xFF', '0xFF']</t>
+    <t>['0xFF', '0x00', '0x0F']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x13', '0x13', '0x13']</t>
+    <t>['0xFF', '0x00', '0x0F']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x07', '0x07', '0x07']</t>
+    <t>['0xFF', '0x00', '0x0F']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>InColorSpace</t>
+    <t>['0xFF', '0x00', '0x0F']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>OutColorSpace</t>
+    <t>['0x4F', '0x55', '0xFB']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>RGB</t>
+    <t>['0x4F', '0x55', '0xFB']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>YCbCr444</t>
+    <t>['0x4F', '0x55', '0xFB']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>YCbCr444</t>
+    <t>['0x01', '0x37', '0xFE']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>RGB</t>
+    <t>['0x01', '0x37', '0xFE']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>x</t>
+    <t>['0x01', '0x37', '0xFE']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>x</t>
+    <t>['0x01', '0x37', '0xFE']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>x</t>
+    <t>['0xFF', '0x00', '0x40']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x0A', '0x0A', '0x0A']</t>
+    <t>['0xFF', '0x00', '0x40']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0xFE', '0x80']</t>
+    <t>['0xFF', '0x00', '0x40']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0x80', '0xF7']</t>
+    <t>['0xFF', '0x00', '0x40']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0xF7', '0x80']</t>
+    <t>['0xFF', '0x00', '0x40']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0xFE', '0x80']</t>
+    <t>Green</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0xFE', '0x80']</t>
+    <t>Blue</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0xFE', '0x80']</t>
+    <t>['0x40', '0x00', '0x80']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0x80', '0xFF']</t>
+    <t>['0x40', '0x00', '0x80']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>32003:1:1</t>
+    <t>['0x01', '0x82', '0x35']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>ConfigResolutionData.xlsx</t>
+    <t>['0x01', '0x82', '0x35']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x10', '0x10', '0x11']</t>
-  </si>
-  <si>
-    <t>['0x0A', '0x0A', '0x1A']</t>
-  </si>
-  <si>
-    <t>['0x13', '0x13', '0x14']</t>
-  </si>
-  <si>
-    <t>['0x80', '0x15', '0x81']</t>
-  </si>
-  <si>
-    <t>['0x80', '0x80', '0x17']</t>
-  </si>
-  <si>
-    <t>['0x07', '0x07', '0x08']</t>
-  </si>
-  <si>
-    <t>['0x80', '0x1C', '0x81']</t>
-  </si>
-  <si>
-    <t>['0x10', '0x80', '0x11']</t>
+    <t>['0x01', '0x82', '0x35']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x3C', '0x75', '0x36']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x3C', '0x75', '0x36']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x3C', '0x75', '0x36']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x3C', '0x75', '0x36']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x3C', '0x75', '0x36']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x10', '0x00', '0xC0']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x10', '0x00', '0xC0']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x10', '0x00', '0xC0']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x10', '0x00', '0xC0']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x10', '0x00', '0xC0']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x39', '0xFF', '0x1C']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x39', '0xFF', '0x1C']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x39', '0xFF', '0x1C']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x39', '0xFF', '0x1C']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xEF', '0x3E', '0x7C']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xEF', '0x3E', '0x7C']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xEF', '0x3E', '0x7C']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xEF', '0x3E', '0x7C']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xFE', '0x37', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xFE', '0x37', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xFE', '0x37', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0xFE', '0x37', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFF', '0x40']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFF', '0x40']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFF', '0x40']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFF', '0x40']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xFF', '0x40']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5079,7 +5231,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5268,6 +5420,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5531,7 +5701,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5585,6 +5755,21 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5978,7 +6163,7 @@
         <v>1405</v>
       </c>
       <c r="AN1" s="17" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="AO1" s="16"/>
     </row>
@@ -6092,19 +6277,19 @@
         <v>25</v>
       </c>
       <c r="AK2" t="s">
+        <v>1427</v>
+      </c>
+      <c r="AL2" s="3" t="s">
         <v>1428</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN2" s="3" t="s">
         <v>1429</v>
       </c>
-      <c r="AM2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>1430</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>1431</v>
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
@@ -9285,7 +9470,7 @@
         <v>30</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="D33" t="s">
         <v>122</v>
@@ -9403,7 +9588,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="D34" t="s">
         <v>124</v>
@@ -12783,7 +12968,7 @@
         <v>203</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="D64" t="s">
         <v>216</v>
@@ -14851,7 +15036,7 @@
         <v>30</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="D82" t="s">
         <v>268</v>
@@ -15661,7 +15846,7 @@
         <v>30</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="D89" t="s">
         <v>291</v>
@@ -27911,10 +28096,10 @@
         <v>30</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="E197">
         <v>1</v>
@@ -29855,10 +30040,10 @@
         <v>30</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="E214">
         <v>1</v>
@@ -30094,7 +30279,7 @@
         <v>657</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="E216">
         <v>1</v>
@@ -31780,7 +31965,7 @@
         <v>697</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="E231">
         <v>1</v>
@@ -31891,10 +32076,10 @@
         <v>30</v>
       </c>
       <c r="C232" s="3" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D232" s="3" t="s">
         <v>1441</v>
-      </c>
-      <c r="D232" s="3" t="s">
-        <v>1442</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -32469,7 +32654,7 @@
         <v>30</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="D237" t="s">
         <v>713</v>
@@ -34039,10 +34224,10 @@
         <v>30</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="E251">
         <v>1</v>
@@ -34271,7 +34456,7 @@
         <v>30</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D253" t="s">
         <v>753</v>
@@ -34853,7 +35038,7 @@
         <v>30</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="D258" t="s">
         <v>766</v>
@@ -37524,7 +37709,7 @@
         <v>835</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="E282">
         <v>1</v>
@@ -39968,7 +40153,7 @@
         <v>901</v>
       </c>
       <c r="D304" s="3" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="E304">
         <v>1</v>
@@ -43717,7 +43902,7 @@
         <v>996</v>
       </c>
       <c r="C338" s="3" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="D338" t="s">
         <v>1009</v>
@@ -47416,7 +47601,7 @@
         <v>30</v>
       </c>
       <c r="C371" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="D371" t="s">
         <v>1100</v>
@@ -58237,7 +58422,7 @@
         <v>30</v>
       </c>
       <c r="C470" s="3" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="D470" t="s">
         <v>1390</v>
@@ -58455,7 +58640,7 @@
         <v>30</v>
       </c>
       <c r="C472" s="3" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="D472" t="s">
         <v>1394</v>
@@ -58583,8 +58768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -58595,31 +58780,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>1498</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1410</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>1451</v>
+      <c r="B3" s="12" t="s">
+        <v>1502</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>1413</v>
@@ -58635,26 +58820,26 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>1420</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>1415</v>
+        <v>1419</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>1503</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -58667,26 +58852,26 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>1497</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>1471</v>
+        <v>1505</v>
       </c>
     </row>
   </sheetData>
@@ -58699,10 +58884,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -58712,702 +58897,1001 @@
     <col min="3" max="3" width="3.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>1469</v>
+        <v>1466</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>1480</v>
+        <v>1476</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>1469</v>
+        <v>1466</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>1481</v>
+        <v>1477</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>1462</v>
+        <v>1459</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>1458</v>
+        <v>1507</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>1508</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>1527</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>1528</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11" t="s">
-        <v>1468</v>
+        <v>1465</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>1465</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>1477</v>
+        <v>1462</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>1515</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>1535</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>1549</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>1463</v>
-      </c>
       <c r="F3" s="11" t="s">
-        <v>1499</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>1490</v>
+        <v>1494</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>1486</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>1518</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>1532</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>1552</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>1489</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>1477</v>
+        <v>1485</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>1510</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>1539</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>1544</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>1500</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>1476</v>
+        <v>1495</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>1522</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>1529</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>1556</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11" t="s">
-        <v>1468</v>
+        <v>1465</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>1465</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>1477</v>
+        <v>1462</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>1516</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>1535</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>1550</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>1463</v>
-      </c>
       <c r="F7" s="11" t="s">
-        <v>1499</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>1492</v>
+        <v>1494</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>1488</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>1520</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>1533</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>1553</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>1478</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>1477</v>
+        <v>1474</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>1511</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>1539</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>1545</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>1501</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>1491</v>
+        <v>1496</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>1487</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>1523</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>1529</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>1557</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>1474</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>1477</v>
+        <v>1470</v>
+      </c>
+      <c r="G10" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>1516</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>1534</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>1551</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="11" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>1502</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>1493</v>
+        <v>1506</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>1489</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>1531</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>1554</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>1482</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>1486</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>1485</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>1463</v>
-      </c>
       <c r="F12" s="11" t="s">
-        <v>1475</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>1477</v>
+        <v>1471</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>1509</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>1540</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>1546</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>1482</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>1486</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>1460</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>1463</v>
-      </c>
       <c r="F13" s="11" t="s">
-        <v>1503</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>1476</v>
+        <v>1498</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>1524</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>1530</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>1557</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>1475</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>1477</v>
+        <v>1471</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>1517</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>1536</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>1548</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>1463</v>
-      </c>
       <c r="F15" s="11" t="s">
-        <v>1503</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>1494</v>
+        <v>1498</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>1490</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>1520</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>1533</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>1555</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>1481</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>1470</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>1485</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>1463</v>
-      </c>
       <c r="F16" s="11" t="s">
-        <v>1475</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>1477</v>
+        <v>1471</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>1512</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>1541</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>1545</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>1470</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>1460</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>1463</v>
-      </c>
       <c r="F17" s="11" t="s">
-        <v>1503</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>1476</v>
+        <v>1498</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>1525</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>1530</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>1558</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>1472</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>1477</v>
+        <v>1468</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>1515</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>1537</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>1551</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="11" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>1502</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>1495</v>
+        <v>1497</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>1491</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>1521</v>
+      </c>
+      <c r="I19" s="22" t="s">
+        <v>1533</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>1555</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>1467</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>1470</v>
-      </c>
       <c r="D20" s="11" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>1479</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>1477</v>
+        <v>1475</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>1510</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>1542</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>1545</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>1482</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>1479</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>1526</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>1530</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>1467</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>1486</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>1463</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>1504</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>1470</v>
-      </c>
       <c r="B22" s="11" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>1472</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>1477</v>
+        <v>1468</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>1516</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>1536</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>1551</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>1502</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>1493</v>
+        <v>1497</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>1489</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>1520</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>1533</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>1553</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>1467</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>1470</v>
-      </c>
       <c r="D24" s="11" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F24" s="11" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>1513</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>1543</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>1464</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>1479</v>
       </c>
-      <c r="G24" s="11" t="s">
-        <v>1477</v>
+      <c r="E25" s="11" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>1492</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>1525</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>1530</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>1558</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>1470</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>1467</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>1470</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>1483</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>1463</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>1504</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>1496</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F26" s="11" t="s">
+        <v>1469</v>
+      </c>
+      <c r="G26" s="18" t="s">
         <v>1473</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>1477</v>
+      <c r="H26" s="20" t="s">
+        <v>1516</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>1538</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>1548</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>1463</v>
-      </c>
       <c r="F27" s="11" t="s">
-        <v>1505</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>1493</v>
+        <v>1500</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>1489</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>1520</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>1533</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>1554</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="E28" s="11" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F28" s="11" t="s">
         <v>1463</v>
       </c>
-      <c r="F28" s="11" t="s">
-        <v>1466</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>1477</v>
+      <c r="G28" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H28" s="20" t="s">
+        <v>1509</v>
+      </c>
+      <c r="I28" s="22" t="s">
+        <v>1543</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>1547</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>1506</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>1476</v>
+        <v>1501</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>1522</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>1530</v>
+      </c>
+      <c r="J29" s="21" t="s">
+        <v>1556</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>1488</v>
+        <v>1484</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F30" s="11" t="s">
+        <v>1469</v>
+      </c>
+      <c r="G30" s="18" t="s">
         <v>1473</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>1477</v>
+      <c r="H30" s="20" t="s">
+        <v>1515</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>1534</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>1551</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
+        <v>1457</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>1460</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="F31" s="11" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>1491</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I31" s="22" t="s">
+        <v>1533</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>1467</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>1461</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>1478</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>1463</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>1505</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>1495</v>
+      <c r="G32" s="18" t="s">
+        <v>1473</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>1514</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>1539</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>1545</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>1470</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>1464</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>1470</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>1482</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>1463</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>1466</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>1477</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>1506</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>1476</v>
+        <v>1501</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>1522</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>1530</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>1560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify log and report to index.html
</commit_message>
<xml_diff>
--- a/hdmi_hdbt_test_suite/ConfigResolutionData.xlsx
+++ b/hdmi_hdbt_test_suite/ConfigResolutionData.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10470" uniqueCount="1540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10470" uniqueCount="1535">
   <si>
     <t>CODE</t>
   </si>
@@ -4754,10 +4754,6 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0xFE', '0x80']</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <t>['0x01', '0x40', '0xFE']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
@@ -4822,10 +4818,6 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0xFE', '0x80']</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <t>['0x39', '0xFF', '0x1C']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
@@ -4862,34 +4854,10 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0x80', '0xEE']</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>['0x80', '0xEE', '0x80']</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <t>['0x80', '0xF4', '0x80']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0x80', '0x80', '0xF4']</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>['0x80', '0xE3', '0x80']</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>['0x80', '0x80', '0xF4']</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.1.156</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <t>['0x80', '0xEB', '0x80']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
@@ -4902,27 +4870,39 @@
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
+    <t>YCbCr420</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>YCbCr420</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0xEB', '0x80']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <t>['0x80', '0x80', '0xEB']</t>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
     <t>['0xEB', '0xEB', '0xEB']</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>['0xEB', '0xEB', '0xEB']</t>
+    <t>DMT1360H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>32002:6:1</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
   <si>
-    <t>YCbCr420</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>YCbCr420</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <t>32003:6:1</t>
+    <t>192.168.1.168</t>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
 </sst>
@@ -5975,8 +5955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS480"/>
   <sheetViews>
-    <sheetView topLeftCell="A439" workbookViewId="0">
-      <selection activeCell="D450" sqref="D450"/>
+    <sheetView topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="C225" sqref="C225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -31370,8 +31350,8 @@
       <c r="B225" t="s">
         <v>30</v>
       </c>
-      <c r="C225" t="s">
-        <v>680</v>
+      <c r="C225" s="7" t="s">
+        <v>1532</v>
       </c>
       <c r="D225" t="s">
         <v>680</v>
@@ -59130,7 +59110,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -59160,7 +59140,7 @@
         <v>1405</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1530</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -59184,7 +59164,7 @@
         <v>1420</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>1539</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -59247,8 +59227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -59258,7 +59238,7 @@
     <col min="3" max="3" width="3.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" customWidth="1"/>
     <col min="7" max="8" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.88671875" customWidth="1"/>
     <col min="10" max="11" width="27.109375" bestFit="1" customWidth="1"/>
@@ -59296,7 +59276,7 @@
         <v>1490</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>1532</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -59327,7 +59307,7 @@
         <v>1496</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>1534</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -59346,19 +59326,19 @@
         <v>1476</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>1528</v>
+        <v>1523</v>
       </c>
       <c r="H3" s="18" t="s">
+        <v>1497</v>
+      </c>
+      <c r="I3" s="19" t="s">
         <v>1498</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="J3" s="20" t="s">
         <v>1499</v>
       </c>
-      <c r="J3" s="20" t="s">
-        <v>1500</v>
-      </c>
       <c r="K3" s="17" t="s">
-        <v>1492</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -59382,13 +59362,13 @@
         <v>1492</v>
       </c>
       <c r="H4" s="18" t="s">
+        <v>1500</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>1501</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="J4" s="20" t="s">
         <v>1502</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>1503</v>
       </c>
       <c r="K4" s="17" t="s">
         <v>1492</v>
@@ -59412,19 +59392,19 @@
         <v>1477</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>1526</v>
+        <v>1530</v>
       </c>
       <c r="H5" s="18" t="s">
+        <v>1503</v>
+      </c>
+      <c r="I5" s="19" t="s">
         <v>1504</v>
       </c>
-      <c r="I5" s="19" t="s">
-        <v>1505</v>
-      </c>
       <c r="J5" s="20" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>1492</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -59478,19 +59458,19 @@
         <v>1476</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>1525</v>
+        <v>1529</v>
       </c>
       <c r="H7" s="18" t="s">
+        <v>1507</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>1498</v>
+      </c>
+      <c r="J7" s="20" t="s">
         <v>1508</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>1499</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>1509</v>
-      </c>
       <c r="K7" s="17" t="s">
-        <v>1492</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -59516,16 +59496,16 @@
         <v>1492</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="I8" s="19" t="s">
+        <v>1501</v>
+      </c>
+      <c r="J8" s="20" t="s">
         <v>1502</v>
       </c>
-      <c r="J8" s="20" t="s">
-        <v>1503</v>
-      </c>
       <c r="K8" s="17" t="s">
-        <v>1535</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -59548,19 +59528,19 @@
         <v>1478</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>1524</v>
+        <v>1525</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>1492</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -59576,7 +59556,7 @@
         <v>1455</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="G10" s="17" t="s">
         <v>1492</v>
@@ -59585,7 +59565,7 @@
         <v>1494</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="J10" s="20" t="s">
         <v>1496</v>
@@ -59607,22 +59587,22 @@
         <v>1455</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>1527</v>
+        <v>1529</v>
       </c>
       <c r="H11" s="18" t="s">
+        <v>1497</v>
+      </c>
+      <c r="I11" s="19" t="s">
         <v>1498</v>
       </c>
-      <c r="I11" s="19" t="s">
-        <v>1499</v>
-      </c>
       <c r="J11" s="20" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -59646,13 +59626,13 @@
         <v>1492</v>
       </c>
       <c r="H12" s="18" t="s">
+        <v>1500</v>
+      </c>
+      <c r="I12" s="19" t="s">
         <v>1501</v>
       </c>
-      <c r="I12" s="19" t="s">
-        <v>1502</v>
-      </c>
       <c r="J12" s="20" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>1492</v>
@@ -59676,19 +59656,19 @@
         <v>1480</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="J13" s="20" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>1492</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -59706,7 +59686,7 @@
         <v>1455</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>1492</v>
@@ -59715,10 +59695,10 @@
         <v>1494</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="J14" s="20" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>1492</v>
@@ -59742,19 +59722,19 @@
         <v>1480</v>
       </c>
       <c r="G15" s="17" t="s">
+        <v>1529</v>
+      </c>
+      <c r="H15" s="18" t="s">
         <v>1497</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="I15" s="19" t="s">
         <v>1498</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="J15" s="20" t="s">
         <v>1499</v>
       </c>
-      <c r="J15" s="20" t="s">
-        <v>1500</v>
-      </c>
       <c r="K15" s="17" t="s">
-        <v>1492</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -59774,19 +59754,19 @@
         <v>1455</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>1492</v>
       </c>
       <c r="H16" s="18" t="s">
+        <v>1500</v>
+      </c>
+      <c r="I16" s="19" t="s">
         <v>1501</v>
       </c>
-      <c r="I16" s="19" t="s">
-        <v>1502</v>
-      </c>
       <c r="J16" s="20" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>1492</v>
@@ -59812,19 +59792,19 @@
         <v>1480</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>1526</v>
+        <v>1530</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -59840,19 +59820,19 @@
         <v>1455</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>1492</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="I18" s="19" t="s">
         <v>1495</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>1492</v>
@@ -59874,19 +59854,19 @@
         <v>1479</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>1514</v>
+        <v>1529</v>
       </c>
       <c r="H19" s="18" t="s">
+        <v>1507</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>1518</v>
+      </c>
+      <c r="J19" s="20" t="s">
         <v>1508</v>
       </c>
-      <c r="I19" s="19" t="s">
-        <v>1520</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>1509</v>
-      </c>
       <c r="K19" s="17" t="s">
-        <v>1492</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -59910,13 +59890,13 @@
         <v>1493</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>1492</v>
@@ -59940,19 +59920,19 @@
         <v>1481</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>1492</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -59970,7 +59950,7 @@
         <v>1455</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>1493</v>
@@ -59982,7 +59962,7 @@
         <v>1495</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>1492</v>
@@ -60006,19 +59986,19 @@
         <v>1479</v>
       </c>
       <c r="G23" s="17" t="s">
+        <v>1529</v>
+      </c>
+      <c r="H23" s="18" t="s">
         <v>1497</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="I23" s="19" t="s">
         <v>1498</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="J23" s="20" t="s">
         <v>1499</v>
       </c>
-      <c r="J23" s="20" t="s">
-        <v>1500</v>
-      </c>
       <c r="K23" s="17" t="s">
-        <v>1492</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -60044,13 +60024,13 @@
         <v>1492</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>1492</v>
@@ -60076,19 +60056,19 @@
         <v>1481</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>1526</v>
+        <v>1530</v>
       </c>
       <c r="H25" s="18" t="s">
+        <v>1503</v>
+      </c>
+      <c r="I25" s="19" t="s">
         <v>1504</v>
       </c>
-      <c r="I25" s="19" t="s">
+      <c r="J25" s="20" t="s">
         <v>1505</v>
       </c>
-      <c r="J25" s="20" t="s">
-        <v>1506</v>
-      </c>
       <c r="K25" s="17" t="s">
-        <v>1492</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -60104,13 +60084,13 @@
         <v>1455</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>1493</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="I26" s="19" t="s">
         <v>1495</v>
@@ -60141,16 +60121,16 @@
         <v>1529</v>
       </c>
       <c r="H27" s="18" t="s">
+        <v>1507</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>1518</v>
+      </c>
+      <c r="J27" s="20" t="s">
         <v>1508</v>
       </c>
-      <c r="I27" s="19" t="s">
-        <v>1520</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>1509</v>
-      </c>
       <c r="K27" s="17" t="s">
-        <v>1492</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -60168,19 +60148,19 @@
         <v>1455</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>1492</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="J28" s="20" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>1492</v>
@@ -60204,19 +60184,19 @@
         <v>1483</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>1526</v>
+        <v>1530</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="J29" s="20" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>1492</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -60243,7 +60223,7 @@
         <v>1494</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>1496</v>
@@ -60270,19 +60250,19 @@
         <v>1482</v>
       </c>
       <c r="G31" s="17" t="s">
+        <v>1529</v>
+      </c>
+      <c r="H31" s="18" t="s">
         <v>1497</v>
       </c>
-      <c r="H31" s="18" t="s">
-        <v>1498</v>
-      </c>
       <c r="I31" s="19" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>1492</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -60302,19 +60282,19 @@
         <v>1455</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>1492</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="J32" s="20" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="K32" s="17" t="s">
         <v>1492</v>
@@ -60340,19 +60320,19 @@
         <v>1483</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>1526</v>
+        <v>1530</v>
       </c>
       <c r="H33" s="18" t="s">
+        <v>1503</v>
+      </c>
+      <c r="I33" s="19" t="s">
         <v>1504</v>
       </c>
-      <c r="I33" s="19" t="s">
+      <c r="J33" s="20" t="s">
         <v>1505</v>
       </c>
-      <c r="J33" s="20" t="s">
-        <v>1506</v>
-      </c>
       <c r="K33" s="17" t="s">
-        <v>1492</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -60362,25 +60342,25 @@
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9" t="s">
-        <v>1536</v>
+        <v>1526</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>1455</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>1492</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="K34" s="17" t="s">
         <v>1492</v>
@@ -60395,7 +60375,7 @@
         <v>1460</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>1537</v>
+        <v>1527</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>1455</v>
@@ -60404,49 +60384,49 @@
         <v>1483</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
       <c r="H35" s="18" t="s">
+        <v>1503</v>
+      </c>
+      <c r="I35" s="19" t="s">
         <v>1504</v>
       </c>
-      <c r="I35" s="19" t="s">
+      <c r="J35" s="20" t="s">
         <v>1505</v>
       </c>
-      <c r="J35" s="20" t="s">
-        <v>1506</v>
-      </c>
       <c r="K35" s="17" t="s">
-        <v>1492</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>1538</v>
+        <v>1528</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>1456</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9" t="s">
-        <v>1536</v>
+        <v>1526</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>1455</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>1492</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="J36" s="20" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="K36" s="17" t="s">
         <v>1492</v>
@@ -60463,7 +60443,7 @@
         <v>1460</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>1537</v>
+        <v>1527</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>1455</v>
@@ -60472,19 +60452,19 @@
         <v>1483</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
       <c r="H37" s="18" t="s">
+        <v>1503</v>
+      </c>
+      <c r="I37" s="19" t="s">
         <v>1504</v>
       </c>
-      <c r="I37" s="19" t="s">
+      <c r="J37" s="20" t="s">
         <v>1505</v>
       </c>
-      <c r="J37" s="20" t="s">
-        <v>1506</v>
-      </c>
       <c r="K37" s="17" t="s">
-        <v>1492</v>
+        <v>1522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>